<commit_message>
pandas#2 심화학습 완료 | groupby, pivot_table 등등
</commit_message>
<xml_diff>
--- a/BoostCourse/머신러닝을 위한 파이썬/03_Data Handling/test.xlsx
+++ b/BoostCourse/머신러닝을 위한 파이썬/03_Data Handling/test.xlsx
@@ -37,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -49,6 +49,27 @@
       <left style="thin"/>
       <right style="thin"/>
       <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top/>
       <bottom style="thin"/>
       <diagonal/>
     </border>
@@ -426,7 +447,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -442,22 +463,12 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>black</t>
+          <t>race</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>hispanic</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>other</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>white</t>
+          <t>earn</t>
         </is>
       </c>
     </row>
@@ -467,39 +478,101 @@
           <t>female</t>
         </is>
       </c>
-      <c r="B2" t="n">
+      <c r="B2" s="1" t="inlineStr">
+        <is>
+          <t>black</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
         <v>26413.2832533842</v>
       </c>
-      <c r="C2" t="n">
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n"/>
+      <c r="B3" s="1" t="inlineStr">
+        <is>
+          <t>hispanic</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
         <v>21217.35209195709</v>
       </c>
-      <c r="D2" t="n">
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n"/>
+      <c r="B4" s="1" t="inlineStr">
+        <is>
+          <t>other</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
         <v>34164.34619665911</v>
       </c>
-      <c r="E2" t="n">
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n"/>
+      <c r="B5" s="1" t="inlineStr">
+        <is>
+          <t>white</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
         <v>23948.24117218976</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="1" t="inlineStr">
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
         <is>
           <t>male</t>
         </is>
       </c>
-      <c r="B3" t="n">
+      <c r="B6" s="1" t="inlineStr">
+        <is>
+          <t>black</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
         <v>31778.72028241918</v>
       </c>
-      <c r="C3" t="n">
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n"/>
+      <c r="B7" s="1" t="inlineStr">
+        <is>
+          <t>hispanic</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
         <v>31818.39067697309</v>
       </c>
-      <c r="D3" t="n">
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n"/>
+      <c r="B8" s="1" t="inlineStr">
+        <is>
+          <t>other</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
         <v>29189.70626633994</v>
       </c>
-      <c r="E3" t="n">
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n"/>
+      <c r="B9" s="1" t="inlineStr">
+        <is>
+          <t>white</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
         <v>48951.73144985256</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A6:A9"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>